<commit_message>
Extract CourseData From CRM file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSource/CRM.xlsx
+++ b/src/main/resources/dataSource/CRM.xlsx
@@ -2288,6 +2288,18 @@
   </si>
   <si>
     <t>OUIJDANE</t>
+  </si>
+  <si>
+    <t>Mle 1</t>
+  </si>
+  <si>
+    <t>Mle 2</t>
+  </si>
+  <si>
+    <t>Mle 3</t>
+  </si>
+  <si>
+    <t>Mle 4</t>
   </si>
 </sst>
 </file>
@@ -2661,7 +2673,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2686,7 +2698,7 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>758</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -2698,7 +2710,7 @@
         <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>759</v>
       </c>
       <c r="L1" t="s">
         <v>14</v>
@@ -2710,7 +2722,7 @@
         <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>10</v>
+        <v>760</v>
       </c>
       <c r="P1" t="s">
         <v>17</v>
@@ -2722,7 +2734,7 @@
         <v>19</v>
       </c>
       <c r="S1" t="s">
-        <v>10</v>
+        <v>761</v>
       </c>
       <c r="T1" t="s">
         <v>20</v>

</xml_diff>